<commit_message>
WIP Version 1.3.0 : leaktest done
</commit_message>
<xml_diff>
--- a/excel_import/leaktest_report_template.xlsx
+++ b/excel_import/leaktest_report_template.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/David's Stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F45CF9DB-5503-4727-BDB9-29AE1BC4DAD9}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{653D43A1-F6F5-4648-B32B-C3E5EB8F6A4C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Part Number :</t>
   </si>
@@ -68,6 +81,12 @@
   </si>
   <si>
     <t>Created By</t>
+  </si>
+  <si>
+    <t>Defect No</t>
+  </si>
+  <si>
+    <t>Defect Desc.</t>
   </si>
 </sst>
 </file>
@@ -252,6 +271,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -260,9 +282,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,10 +600,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M11"/>
+  <dimension ref="B1:O11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -592,20 +611,22 @@
     <col min="1" max="1" width="5.140625" style="22" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" style="24" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" style="26" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" style="21" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="21" customWidth="1"/>
-    <col min="13" max="13" width="22.7109375" style="21" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="22" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="22"/>
+    <col min="5" max="5" width="12.7109375" style="25" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="25" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="25" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="25" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="25" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="26" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" style="21" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="21" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" style="21" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="22" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="4"/>
       <c r="C1" s="8"/>
       <c r="D1" s="4"/>
@@ -617,25 +638,29 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="2:13" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="2:15" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
       <c r="J2" s="29"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="20"/>
-    </row>
-    <row r="3" spans="2:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="29"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="20"/>
+    </row>
+    <row r="3" spans="2:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
@@ -647,10 +672,12 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="2:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="2:15" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>7</v>
       </c>
@@ -662,10 +689,12 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="2:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>0</v>
       </c>
@@ -673,15 +702,17 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="15"/>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="M5" s="13"/>
-    </row>
-    <row r="6" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="13"/>
+      <c r="O5" s="13"/>
+    </row>
+    <row r="6" spans="2:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>1</v>
       </c>
@@ -689,15 +720,17 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="30"/>
-      <c r="M6" s="5"/>
-    </row>
-    <row r="7" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="27"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -709,9 +742,11 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="2:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>2</v>
       </c>
@@ -722,44 +757,50 @@
         <v>9</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="L8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="67" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>